<commit_message>
added dimentions, next changes will be a rev 2
</commit_message>
<xml_diff>
--- a/Documentation/BMS_2021_BOM.xlsx
+++ b/Documentation/BMS_2021_BOM.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxwe\Documents\GitHub\BMS_Hardware\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C17865-9A88-4A44-A0E4-239D13323BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F673F57-CE45-4DCD-9C7E-1FFA5A42C6AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8655" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MRDT BOM Template.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1059,6 +1060,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1067,9 +1071,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1392,8 +1393,8 @@
   </sheetPr>
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2139,7 +2140,7 @@
       <c r="K21" s="9">
         <v>0.69</v>
       </c>
-      <c r="N21" s="53" t="s">
+      <c r="N21" s="50" t="s">
         <v>212</v>
       </c>
     </row>
@@ -2319,13 +2320,13 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="51" t="s">
+      <c r="C27" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="52" t="s">
+      <c r="D27" s="53" t="s">
         <v>88</v>
       </c>
       <c r="F27" s="15" t="s">
@@ -2351,9 +2352,9 @@
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="52"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="53"/>
       <c r="F28" s="15" t="s">
         <v>207</v>
       </c>
@@ -2377,9 +2378,9 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="52"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="53"/>
       <c r="F29" s="10" t="s">
         <v>206</v>
       </c>
@@ -2771,7 +2772,7 @@
       <c r="K40" s="9">
         <v>0.31</v>
       </c>
-      <c r="N40" s="53" t="s">
+      <c r="N40" s="50" t="s">
         <v>216</v>
       </c>
     </row>

</xml_diff>